<commit_message>
Exe 16 - axb
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/9.Cac-van-de-mo-rong.xlsx
+++ b/me/1.Lap-trinh-python/9.Cac-van-de-mo-rong.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708F54A1-E51D-C44E-9645-83F6F7328DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1DAD6C-00CD-A54B-B2DF-D62A561C63D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="920" windowWidth="33800" windowHeight="18400" activeTab="3" xr2:uid="{472041F3-94B6-BA44-8755-3BBFF041A0A3}"/>
+    <workbookView xWindow="960" yWindow="880" windowWidth="33800" windowHeight="18400" activeTab="4" xr2:uid="{472041F3-94B6-BA44-8755-3BBFF041A0A3}"/>
   </bookViews>
   <sheets>
     <sheet name="name" sheetId="1" r:id="rId1"/>
     <sheet name="Local - global" sheetId="2" r:id="rId2"/>
     <sheet name="Re 01" sheetId="3" r:id="rId3"/>
     <sheet name="Re 02" sheetId="4" r:id="rId4"/>
+    <sheet name="Exe 16 - axb" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="181">
   <si>
     <t>構成</t>
   </si>
@@ -412,9 +413,6 @@
     <t>python3 03_re_01.py</t>
   </si>
   <si>
-    <t>Kiểm tra xem pattern có ở đầu chuỗi text hay không</t>
-  </si>
-  <si>
     <t>text    = "123 abc xabc 456"</t>
   </si>
   <si>
@@ -521,13 +519,116 @@
   </si>
   <si>
     <t>03_re_05.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_16_axb.py</t>
+  </si>
+  <si>
+    <t>exe_16_axb.py</t>
+  </si>
+  <si>
+    <t># Input     : Kiểm tra mẫu chuỗi bất kỳ có thỏa mãn: Bắt đầu bằng a và kết thúc bằng b</t>
+  </si>
+  <si>
+    <t># Output    : Match hoặc Not match</t>
+  </si>
+  <si>
+    <t># python regular expression match vs search</t>
+  </si>
+  <si>
+    <t>import re</t>
+  </si>
+  <si>
+    <t>def checkAxB(text):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    patterns = '^a.*b$'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if re.match(patterns,  text):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return 'Match!'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    else:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return('Not match!')</t>
+  </si>
+  <si>
+    <t>print(checkAxB("ab"))</t>
+  </si>
+  <si>
+    <t>print(checkAxB("1ab"))</t>
+  </si>
+  <si>
+    <t>print(checkAxB("ab1"))</t>
+  </si>
+  <si>
+    <t>print(checkAxB("1ab1"))</t>
+  </si>
+  <si>
+    <t>print(checkAxB("adsdsdasda1231321b"))</t>
+  </si>
+  <si>
+    <t>python3 exe_16_axb.py</t>
+  </si>
+  <si>
+    <t>Bắt đầu là a và kết thúc là b</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">search() kiểm tra chuỗi text có </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>chứa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern hay không</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kiểm tra xem pattern có ở </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>đầu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chuỗi text hay không. So sánh từ ngay vị trí bắt đầu</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -556,6 +657,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -688,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -717,6 +823,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1716,6 +1823,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>79790</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>46544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>641133</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>39896</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C04ADB3-01FA-5476-98A2-6E9E8F9BA050}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="904293" y="22308115"/>
+          <a:ext cx="8806369" cy="1436231"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4268,8 +4424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF812D9-6BE9-D24E-A2E0-24511D7FDF00}">
   <dimension ref="A3:O182"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView topLeftCell="A82" zoomScale="125" workbookViewId="0">
+      <selection activeCell="M98" sqref="M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4872,7 +5028,7 @@
       <c r="B55" s="5"/>
       <c r="C55" s="1"/>
       <c r="D55" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="6"/>
@@ -5263,7 +5419,7 @@
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="15"/>
       <c r="B90" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H90" s="16"/>
       <c r="N90" s="16"/>
@@ -5286,7 +5442,7 @@
         <v>71</v>
       </c>
       <c r="J92" t="s">
-        <v>124</v>
+        <v>180</v>
       </c>
       <c r="N92" s="16"/>
       <c r="O92" s="16"/>
@@ -5312,7 +5468,7 @@
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="15"/>
       <c r="B95" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H95" s="16"/>
       <c r="N95" s="16"/>
@@ -5419,7 +5575,7 @@
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="15"/>
       <c r="B109" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C109" s="13"/>
       <c r="D109" s="13"/>
@@ -5475,7 +5631,7 @@
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="15"/>
       <c r="B114" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H114" s="16"/>
       <c r="L114" s="16"/>
@@ -5484,7 +5640,7 @@
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" s="15"/>
       <c r="B115" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H115" s="16"/>
       <c r="L115" s="16"/>
@@ -5527,7 +5683,7 @@
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" s="15"/>
       <c r="B120" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H120" s="16"/>
       <c r="L120" s="16"/>
@@ -5661,7 +5817,7 @@
     <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" s="15"/>
       <c r="B135" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C135" s="13"/>
       <c r="D135" s="13"/>
@@ -5717,7 +5873,7 @@
     <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" s="15"/>
       <c r="B140" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H140" s="16"/>
       <c r="L140" s="16"/>
@@ -5726,7 +5882,7 @@
     <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" s="15"/>
       <c r="B141" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H141" s="16"/>
       <c r="L141" s="16"/>
@@ -5769,7 +5925,7 @@
     <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" s="15"/>
       <c r="B146" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H146" s="16"/>
       <c r="L146" s="16"/>
@@ -5911,7 +6067,7 @@
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B162" s="13"/>
       <c r="C162" s="13"/>
@@ -5946,21 +6102,21 @@
     <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165" s="15"/>
       <c r="B165" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E165" s="16"/>
       <c r="F165" t="s">
         <v>71</v>
       </c>
       <c r="G165" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N165" s="16"/>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166" s="15"/>
       <c r="B166" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E166" s="16"/>
       <c r="N166" s="16"/>
@@ -6006,7 +6162,7 @@
     <row r="172" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A172" s="15"/>
       <c r="B172" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E172" s="16"/>
       <c r="N172" s="16"/>
@@ -6030,7 +6186,7 @@
     <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176" s="15"/>
       <c r="B176" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C176" s="13"/>
       <c r="D176" s="13"/>
@@ -6111,8 +6267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE7EA81-C65D-AE43-BEF4-A04FBFABC41A}">
   <dimension ref="A3:P180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="150" workbookViewId="0">
-      <selection activeCell="L65" sqref="L65"/>
+    <sheetView topLeftCell="A81" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K89" sqref="K89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6711,7 +6867,7 @@
       <c r="B55" s="5"/>
       <c r="C55" s="1"/>
       <c r="D55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="6"/>
@@ -6721,7 +6877,7 @@
       <c r="B56" s="5"/>
       <c r="C56" s="1"/>
       <c r="D56" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="6"/>
@@ -6737,7 +6893,7 @@
       <c r="B57" s="5"/>
       <c r="C57" s="1"/>
       <c r="D57" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="6"/>
@@ -6753,7 +6909,7 @@
       <c r="B58" s="5"/>
       <c r="C58" s="1"/>
       <c r="D58" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="6"/>
@@ -7057,7 +7213,7 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -7145,7 +7301,7 @@
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="15"/>
       <c r="B93" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H93" s="16"/>
       <c r="N93" s="16"/>
@@ -7154,7 +7310,7 @@
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="15"/>
       <c r="B94" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H94" s="16"/>
       <c r="N94" s="16"/>
@@ -7170,23 +7326,29 @@
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="15"/>
       <c r="B96" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H96" s="16"/>
+      <c r="I96" t="s">
+        <v>71</v>
+      </c>
+      <c r="J96" t="s">
+        <v>179</v>
+      </c>
       <c r="N96" s="16"/>
       <c r="P96" s="16"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="15"/>
       <c r="B97" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H97" s="16"/>
       <c r="I97" t="s">
         <v>71</v>
       </c>
       <c r="J97" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N97" s="16"/>
       <c r="P97" s="16"/>
@@ -7203,7 +7365,7 @@
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="15"/>
       <c r="B99" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H99" s="16"/>
       <c r="N99" s="16"/>
@@ -7236,7 +7398,7 @@
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" s="15"/>
       <c r="B103" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C103" s="13"/>
       <c r="D103" s="13"/>
@@ -7325,7 +7487,7 @@
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="15"/>
       <c r="B112" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C112" s="13"/>
       <c r="D112" s="13"/>
@@ -7384,7 +7546,7 @@
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" s="15"/>
       <c r="B117" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H117" s="16"/>
       <c r="O117" s="16"/>
@@ -7393,7 +7555,7 @@
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" s="15"/>
       <c r="B118" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H118" s="16"/>
       <c r="O118" s="16"/>
@@ -7402,7 +7564,7 @@
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" s="15"/>
       <c r="B119" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H119" s="16"/>
       <c r="O119" s="16"/>
@@ -7418,7 +7580,7 @@
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="15"/>
       <c r="B121" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H121" s="16"/>
       <c r="O121" s="16"/>
@@ -7427,7 +7589,7 @@
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="15"/>
       <c r="B122" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H122" s="16"/>
       <c r="O122" s="16"/>
@@ -7445,7 +7607,7 @@
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" s="15"/>
       <c r="B124" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H124" s="16"/>
       <c r="O124" s="16"/>
@@ -7478,7 +7640,7 @@
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="15"/>
       <c r="B128" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C128" s="13"/>
       <c r="D128" s="13"/>
@@ -7586,7 +7748,7 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B139" s="13"/>
       <c r="C139" s="13"/>
@@ -7622,7 +7784,7 @@
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="15"/>
       <c r="B142" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F142" s="16"/>
       <c r="N142" s="16"/>
@@ -7630,7 +7792,7 @@
     <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="15"/>
       <c r="B143" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F143" s="16"/>
       <c r="N143" s="16"/>
@@ -7644,14 +7806,14 @@
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="15"/>
       <c r="B145" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F145" s="16"/>
       <c r="G145" t="s">
         <v>71</v>
       </c>
       <c r="H145" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N145" s="16"/>
     </row>
@@ -7682,7 +7844,7 @@
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" s="15"/>
       <c r="B149" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F149" s="16"/>
       <c r="N149" s="16"/>
@@ -7707,7 +7869,7 @@
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" s="15"/>
       <c r="B153" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C153" s="13"/>
       <c r="D153" s="13"/>
@@ -7780,7 +7942,7 @@
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B162" s="13"/>
       <c r="C162" s="13"/>
@@ -7805,133 +7967,62 @@
       <c r="C163" s="13"/>
       <c r="D163" s="13"/>
       <c r="E163" s="14"/>
-      <c r="F163" s="26"/>
-      <c r="G163" s="26"/>
-      <c r="H163" s="26"/>
-      <c r="I163" s="26"/>
-      <c r="J163" s="26"/>
-      <c r="K163" s="26"/>
-      <c r="L163" s="26"/>
-      <c r="M163" s="26"/>
-      <c r="N163" s="26"/>
       <c r="O163" s="16"/>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" s="15"/>
       <c r="B164" s="15"/>
-      <c r="C164" s="26"/>
-      <c r="D164" s="26"/>
       <c r="E164" s="16"/>
-      <c r="F164" s="26"/>
-      <c r="G164" s="26"/>
-      <c r="H164" s="26"/>
-      <c r="I164" s="26"/>
-      <c r="J164" s="26"/>
-      <c r="K164" s="26"/>
-      <c r="L164" s="26"/>
-      <c r="M164" s="26"/>
-      <c r="N164" s="26"/>
       <c r="O164" s="16"/>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" s="15"/>
       <c r="B165" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C165" s="26"/>
-      <c r="D165" s="26"/>
+        <v>152</v>
+      </c>
       <c r="E165" s="16"/>
-      <c r="F165" s="26" t="s">
+      <c r="F165" t="s">
         <v>71</v>
       </c>
-      <c r="G165" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="H165" s="26"/>
-      <c r="I165" s="26"/>
-      <c r="J165" s="26"/>
-      <c r="K165" s="26"/>
-      <c r="L165" s="26"/>
-      <c r="M165" s="26"/>
-      <c r="N165" s="26"/>
+      <c r="G165" t="s">
+        <v>158</v>
+      </c>
       <c r="O165" s="16"/>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" s="15"/>
       <c r="B166" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C166" s="26"/>
-      <c r="D166" s="26"/>
+        <v>153</v>
+      </c>
       <c r="E166" s="16"/>
-      <c r="F166" s="26"/>
-      <c r="G166" s="26"/>
-      <c r="H166" s="26"/>
-      <c r="I166" s="26"/>
-      <c r="J166" s="26"/>
-      <c r="K166" s="26"/>
-      <c r="L166" s="26"/>
-      <c r="M166" s="26"/>
-      <c r="N166" s="26"/>
       <c r="O166" s="16"/>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" s="15"/>
       <c r="B167" s="15"/>
-      <c r="C167" s="26"/>
-      <c r="D167" s="26"/>
       <c r="E167" s="16"/>
-      <c r="F167" s="26"/>
-      <c r="G167" s="26"/>
-      <c r="H167" s="26"/>
-      <c r="I167" s="26"/>
-      <c r="J167" s="26"/>
-      <c r="K167" s="26"/>
-      <c r="L167" s="26"/>
-      <c r="M167" s="26"/>
-      <c r="N167" s="26"/>
       <c r="O167" s="16"/>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" s="15"/>
       <c r="B168" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="C168" s="26"/>
-      <c r="D168" s="26"/>
+        <v>154</v>
+      </c>
       <c r="E168" s="16"/>
-      <c r="F168" s="26" t="s">
+      <c r="F168" t="s">
         <v>71</v>
       </c>
-      <c r="G168" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="H168" s="26"/>
-      <c r="I168" s="26"/>
-      <c r="J168" s="26"/>
-      <c r="K168" s="26"/>
-      <c r="L168" s="26"/>
-      <c r="M168" s="26"/>
-      <c r="N168" s="26"/>
+      <c r="G168" t="s">
+        <v>157</v>
+      </c>
       <c r="O168" s="16"/>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" s="15"/>
       <c r="B169" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C169" s="26"/>
-      <c r="D169" s="26"/>
+        <v>155</v>
+      </c>
       <c r="E169" s="16"/>
-      <c r="F169" s="26"/>
-      <c r="G169" s="26"/>
-      <c r="H169" s="26"/>
-      <c r="I169" s="26"/>
-      <c r="J169" s="26"/>
-      <c r="K169" s="26"/>
-      <c r="L169" s="26"/>
-      <c r="M169" s="26"/>
-      <c r="N169" s="26"/>
       <c r="O169" s="16"/>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.2">
@@ -7940,55 +8031,20 @@
       <c r="C170" s="18"/>
       <c r="D170" s="18"/>
       <c r="E170" s="19"/>
-      <c r="F170" s="26"/>
-      <c r="G170" s="26"/>
-      <c r="H170" s="26"/>
-      <c r="I170" s="26"/>
-      <c r="J170" s="26"/>
-      <c r="K170" s="26"/>
-      <c r="L170" s="26"/>
-      <c r="M170" s="26"/>
-      <c r="N170" s="26"/>
       <c r="O170" s="16"/>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" s="15"/>
-      <c r="B171" s="26"/>
-      <c r="C171" s="26"/>
-      <c r="D171" s="26"/>
-      <c r="E171" s="26"/>
-      <c r="F171" s="26"/>
-      <c r="G171" s="26"/>
-      <c r="H171" s="26"/>
-      <c r="I171" s="26"/>
-      <c r="J171" s="26"/>
-      <c r="K171" s="26"/>
-      <c r="L171" s="26"/>
-      <c r="M171" s="26"/>
-      <c r="N171" s="26"/>
       <c r="O171" s="16"/>
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" s="15"/>
-      <c r="B172" s="26"/>
-      <c r="C172" s="26"/>
-      <c r="D172" s="26"/>
-      <c r="E172" s="26"/>
-      <c r="F172" s="26"/>
-      <c r="G172" s="26"/>
-      <c r="H172" s="26"/>
-      <c r="I172" s="26"/>
-      <c r="J172" s="26"/>
-      <c r="K172" s="26"/>
-      <c r="L172" s="26"/>
-      <c r="M172" s="26"/>
-      <c r="N172" s="26"/>
       <c r="O172" s="16"/>
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" s="15"/>
       <c r="B173" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C173" s="13"/>
       <c r="D173" s="13"/>
@@ -8007,85 +8063,30 @@
     <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" s="15"/>
       <c r="B174" s="15"/>
-      <c r="C174" s="26"/>
-      <c r="D174" s="26"/>
-      <c r="E174" s="26"/>
-      <c r="F174" s="26"/>
-      <c r="G174" s="26"/>
-      <c r="H174" s="26"/>
-      <c r="I174" s="26"/>
-      <c r="J174" s="26"/>
-      <c r="K174" s="26"/>
-      <c r="L174" s="26"/>
-      <c r="M174" s="26"/>
       <c r="N174" s="16"/>
       <c r="O174" s="16"/>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" s="15"/>
       <c r="B175" s="15"/>
-      <c r="C175" s="26"/>
-      <c r="D175" s="26"/>
-      <c r="E175" s="26"/>
-      <c r="F175" s="26"/>
-      <c r="G175" s="26"/>
-      <c r="H175" s="26"/>
-      <c r="I175" s="26"/>
-      <c r="J175" s="26"/>
-      <c r="K175" s="26"/>
-      <c r="L175" s="26"/>
-      <c r="M175" s="26"/>
       <c r="N175" s="16"/>
       <c r="O175" s="16"/>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" s="15"/>
       <c r="B176" s="15"/>
-      <c r="C176" s="26"/>
-      <c r="D176" s="26"/>
-      <c r="E176" s="26"/>
-      <c r="F176" s="26"/>
-      <c r="G176" s="26"/>
-      <c r="H176" s="26"/>
-      <c r="I176" s="26"/>
-      <c r="J176" s="26"/>
-      <c r="K176" s="26"/>
-      <c r="L176" s="26"/>
-      <c r="M176" s="26"/>
       <c r="N176" s="16"/>
       <c r="O176" s="16"/>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" s="15"/>
       <c r="B177" s="15"/>
-      <c r="C177" s="26"/>
-      <c r="D177" s="26"/>
-      <c r="E177" s="26"/>
-      <c r="F177" s="26"/>
-      <c r="G177" s="26"/>
-      <c r="H177" s="26"/>
-      <c r="I177" s="26"/>
-      <c r="J177" s="26"/>
-      <c r="K177" s="26"/>
-      <c r="L177" s="26"/>
-      <c r="M177" s="26"/>
       <c r="N177" s="16"/>
       <c r="O177" s="16"/>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" s="15"/>
       <c r="B178" s="15"/>
-      <c r="C178" s="26"/>
-      <c r="D178" s="26"/>
-      <c r="E178" s="26"/>
-      <c r="F178" s="26"/>
-      <c r="G178" s="26"/>
-      <c r="H178" s="26"/>
-      <c r="I178" s="26"/>
-      <c r="J178" s="26"/>
-      <c r="K178" s="26"/>
-      <c r="L178" s="26"/>
-      <c r="M178" s="26"/>
       <c r="N178" s="16"/>
       <c r="O178" s="16"/>
     </row>
@@ -8127,4 +8128,1402 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DAD38-D54D-9F45-8003-4333ED54CE92}">
+  <dimension ref="A3:M117"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="191" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="1"/>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="1"/>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="1"/>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="5"/>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="5"/>
+      <c r="D39" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="5"/>
+      <c r="D40" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="5"/>
+      <c r="D41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="1"/>
+      <c r="D43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="1"/>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="1"/>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="1"/>
+      <c r="D46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="1"/>
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="1"/>
+      <c r="D48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="1"/>
+      <c r="D49" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="1"/>
+      <c r="D50" t="s">
+        <v>47</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="1"/>
+      <c r="D52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="1"/>
+      <c r="D53" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="1"/>
+      <c r="D54" t="s">
+        <v>111</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="1"/>
+      <c r="D55" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="1"/>
+      <c r="D59" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="1"/>
+      <c r="D62" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="1"/>
+      <c r="D63" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="1"/>
+      <c r="D64" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="1"/>
+      <c r="D65" t="s">
+        <v>53</v>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="1"/>
+      <c r="D66" t="s">
+        <v>54</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="5"/>
+      <c r="C80" t="s">
+        <v>68</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="5"/>
+      <c r="C81" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="B82" s="5"/>
+      <c r="C82" t="s">
+        <v>70</v>
+      </c>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H83" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="1"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A87" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="13"/>
+      <c r="M87" s="14"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A88" s="15"/>
+      <c r="B88" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="27"/>
+      <c r="J88" s="27"/>
+      <c r="K88" s="27"/>
+      <c r="L88" s="27"/>
+      <c r="M88" s="16"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A89" s="15"/>
+      <c r="B89" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="16"/>
+      <c r="I89" s="27"/>
+      <c r="J89" s="27"/>
+      <c r="K89" s="27"/>
+      <c r="L89" s="27"/>
+      <c r="M89" s="16"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A90" s="15"/>
+      <c r="B90" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C90" s="27"/>
+      <c r="D90" s="27"/>
+      <c r="E90" s="27"/>
+      <c r="F90" s="27"/>
+      <c r="G90" s="27"/>
+      <c r="H90" s="16"/>
+      <c r="I90" s="27"/>
+      <c r="J90" s="27"/>
+      <c r="K90" s="27"/>
+      <c r="L90" s="27"/>
+      <c r="M90" s="16"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A91" s="15"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="27"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="27"/>
+      <c r="J91" s="27"/>
+      <c r="K91" s="27"/>
+      <c r="L91" s="27"/>
+      <c r="M91" s="16"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" s="15"/>
+      <c r="B92" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="27"/>
+      <c r="F92" s="27"/>
+      <c r="G92" s="27"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="27"/>
+      <c r="J92" s="27"/>
+      <c r="K92" s="27"/>
+      <c r="L92" s="27"/>
+      <c r="M92" s="16"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A93" s="15"/>
+      <c r="B93" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="27"/>
+      <c r="G93" s="27"/>
+      <c r="H93" s="16"/>
+      <c r="I93" s="27"/>
+      <c r="J93" s="27"/>
+      <c r="K93" s="27"/>
+      <c r="L93" s="27"/>
+      <c r="M93" s="16"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" s="15"/>
+      <c r="B94" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="27"/>
+      <c r="F94" s="27"/>
+      <c r="G94" s="27"/>
+      <c r="H94" s="16"/>
+      <c r="I94" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="J94" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="K94" s="27"/>
+      <c r="L94" s="27"/>
+      <c r="M94" s="16"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A95" s="15"/>
+      <c r="B95" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="27"/>
+      <c r="G95" s="27"/>
+      <c r="H95" s="16"/>
+      <c r="I95" s="27"/>
+      <c r="J95" s="27"/>
+      <c r="K95" s="27"/>
+      <c r="L95" s="27"/>
+      <c r="M95" s="16"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A96" s="15"/>
+      <c r="B96" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C96" s="27"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="27"/>
+      <c r="G96" s="27"/>
+      <c r="H96" s="16"/>
+      <c r="I96" s="27"/>
+      <c r="J96" s="27"/>
+      <c r="K96" s="27"/>
+      <c r="L96" s="27"/>
+      <c r="M96" s="16"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A97" s="15"/>
+      <c r="B97" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C97" s="27"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="27"/>
+      <c r="F97" s="27"/>
+      <c r="G97" s="27"/>
+      <c r="H97" s="16"/>
+      <c r="I97" s="27"/>
+      <c r="J97" s="27"/>
+      <c r="K97" s="27"/>
+      <c r="L97" s="27"/>
+      <c r="M97" s="16"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A98" s="15"/>
+      <c r="B98" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="27"/>
+      <c r="H98" s="16"/>
+      <c r="I98" s="27"/>
+      <c r="J98" s="27"/>
+      <c r="K98" s="27"/>
+      <c r="L98" s="27"/>
+      <c r="M98" s="16"/>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A99" s="15"/>
+      <c r="B99" s="15"/>
+      <c r="C99" s="27"/>
+      <c r="D99" s="27"/>
+      <c r="E99" s="27"/>
+      <c r="F99" s="27"/>
+      <c r="G99" s="27"/>
+      <c r="H99" s="16"/>
+      <c r="I99" s="27"/>
+      <c r="J99" s="27"/>
+      <c r="K99" s="27"/>
+      <c r="L99" s="27"/>
+      <c r="M99" s="16"/>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A100" s="15"/>
+      <c r="B100" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="27"/>
+      <c r="H100" s="16"/>
+      <c r="I100" s="27"/>
+      <c r="J100" s="27"/>
+      <c r="K100" s="27"/>
+      <c r="L100" s="27"/>
+      <c r="M100" s="16"/>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A101" s="15"/>
+      <c r="B101" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="27"/>
+      <c r="G101" s="27"/>
+      <c r="H101" s="16"/>
+      <c r="I101" s="27"/>
+      <c r="J101" s="27"/>
+      <c r="K101" s="27"/>
+      <c r="L101" s="27"/>
+      <c r="M101" s="16"/>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A102" s="15"/>
+      <c r="B102" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C102" s="27"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27"/>
+      <c r="G102" s="27"/>
+      <c r="H102" s="16"/>
+      <c r="I102" s="27"/>
+      <c r="J102" s="27"/>
+      <c r="K102" s="27"/>
+      <c r="L102" s="27"/>
+      <c r="M102" s="16"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A103" s="15"/>
+      <c r="B103" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C103" s="27"/>
+      <c r="D103" s="27"/>
+      <c r="E103" s="27"/>
+      <c r="F103" s="27"/>
+      <c r="G103" s="27"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="27"/>
+      <c r="J103" s="27"/>
+      <c r="K103" s="27"/>
+      <c r="L103" s="27"/>
+      <c r="M103" s="16"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A104" s="15"/>
+      <c r="B104" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C104" s="27"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="27"/>
+      <c r="G104" s="27"/>
+      <c r="H104" s="16"/>
+      <c r="I104" s="27"/>
+      <c r="J104" s="27"/>
+      <c r="K104" s="27"/>
+      <c r="L104" s="27"/>
+      <c r="M104" s="16"/>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A105" s="15"/>
+      <c r="B105" s="17"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="19"/>
+      <c r="I105" s="27"/>
+      <c r="J105" s="27"/>
+      <c r="K105" s="27"/>
+      <c r="L105" s="27"/>
+      <c r="M105" s="16"/>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A106" s="15"/>
+      <c r="B106" s="27"/>
+      <c r="C106" s="27"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="27"/>
+      <c r="H106" s="27"/>
+      <c r="I106" s="27"/>
+      <c r="J106" s="27"/>
+      <c r="K106" s="27"/>
+      <c r="L106" s="27"/>
+      <c r="M106" s="16"/>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A107" s="15"/>
+      <c r="B107" s="27"/>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="27"/>
+      <c r="G107" s="27"/>
+      <c r="H107" s="27"/>
+      <c r="I107" s="27"/>
+      <c r="J107" s="27"/>
+      <c r="K107" s="27"/>
+      <c r="L107" s="27"/>
+      <c r="M107" s="16"/>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A108" s="15"/>
+      <c r="B108" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="13"/>
+      <c r="K108" s="13"/>
+      <c r="L108" s="14"/>
+      <c r="M108" s="16"/>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A109" s="15"/>
+      <c r="B109" s="15"/>
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="27"/>
+      <c r="I109" s="27"/>
+      <c r="J109" s="27"/>
+      <c r="K109" s="27"/>
+      <c r="L109" s="16"/>
+      <c r="M109" s="16"/>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A110" s="15"/>
+      <c r="B110" s="15"/>
+      <c r="C110" s="27"/>
+      <c r="D110" s="27"/>
+      <c r="E110" s="27"/>
+      <c r="F110" s="27"/>
+      <c r="G110" s="27"/>
+      <c r="H110" s="27"/>
+      <c r="I110" s="27"/>
+      <c r="J110" s="27"/>
+      <c r="K110" s="27"/>
+      <c r="L110" s="16"/>
+      <c r="M110" s="16"/>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A111" s="15"/>
+      <c r="B111" s="15"/>
+      <c r="C111" s="27"/>
+      <c r="D111" s="27"/>
+      <c r="E111" s="27"/>
+      <c r="F111" s="27"/>
+      <c r="G111" s="27"/>
+      <c r="H111" s="27"/>
+      <c r="I111" s="27"/>
+      <c r="J111" s="27"/>
+      <c r="K111" s="27"/>
+      <c r="L111" s="16"/>
+      <c r="M111" s="16"/>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A112" s="15"/>
+      <c r="B112" s="15"/>
+      <c r="C112" s="27"/>
+      <c r="D112" s="27"/>
+      <c r="E112" s="27"/>
+      <c r="F112" s="27"/>
+      <c r="G112" s="27"/>
+      <c r="H112" s="27"/>
+      <c r="I112" s="27"/>
+      <c r="J112" s="27"/>
+      <c r="K112" s="27"/>
+      <c r="L112" s="16"/>
+      <c r="M112" s="16"/>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A113" s="15"/>
+      <c r="B113" s="15"/>
+      <c r="C113" s="27"/>
+      <c r="D113" s="27"/>
+      <c r="E113" s="27"/>
+      <c r="F113" s="27"/>
+      <c r="G113" s="27"/>
+      <c r="H113" s="27"/>
+      <c r="I113" s="27"/>
+      <c r="J113" s="27"/>
+      <c r="K113" s="27"/>
+      <c r="L113" s="16"/>
+      <c r="M113" s="16"/>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A114" s="15"/>
+      <c r="B114" s="15"/>
+      <c r="C114" s="27"/>
+      <c r="D114" s="27"/>
+      <c r="E114" s="27"/>
+      <c r="F114" s="27"/>
+      <c r="G114" s="27"/>
+      <c r="H114" s="27"/>
+      <c r="I114" s="27"/>
+      <c r="J114" s="27"/>
+      <c r="K114" s="27"/>
+      <c r="L114" s="16"/>
+      <c r="M114" s="16"/>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A115" s="15"/>
+      <c r="B115" s="15"/>
+      <c r="C115" s="27"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="27"/>
+      <c r="H115" s="27"/>
+      <c r="I115" s="27"/>
+      <c r="J115" s="27"/>
+      <c r="K115" s="27"/>
+      <c r="L115" s="16"/>
+      <c r="M115" s="16"/>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116" s="15"/>
+      <c r="B116" s="17"/>
+      <c r="C116" s="18"/>
+      <c r="D116" s="18"/>
+      <c r="E116" s="18"/>
+      <c r="F116" s="18"/>
+      <c r="G116" s="18"/>
+      <c r="H116" s="18"/>
+      <c r="I116" s="18"/>
+      <c r="J116" s="18"/>
+      <c r="K116" s="18"/>
+      <c r="L116" s="19"/>
+      <c r="M116" s="16"/>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A117" s="17"/>
+      <c r="B117" s="18"/>
+      <c r="C117" s="18"/>
+      <c r="D117" s="18"/>
+      <c r="E117" s="18"/>
+      <c r="F117" s="18"/>
+      <c r="G117" s="18"/>
+      <c r="H117" s="18"/>
+      <c r="I117" s="18"/>
+      <c r="J117" s="18"/>
+      <c r="K117" s="18"/>
+      <c r="L117" s="18"/>
+      <c r="M117" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exe 17 - Find number
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/9.Cac-van-de-mo-rong.xlsx
+++ b/me/1.Lap-trinh-python/9.Cac-van-de-mo-rong.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1DAD6C-00CD-A54B-B2DF-D62A561C63D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFA057D-FD60-6649-8DCD-962AD7254D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="880" windowWidth="33800" windowHeight="18400" activeTab="4" xr2:uid="{472041F3-94B6-BA44-8755-3BBFF041A0A3}"/>
+    <workbookView xWindow="960" yWindow="820" windowWidth="33800" windowHeight="18400" activeTab="5" xr2:uid="{472041F3-94B6-BA44-8755-3BBFF041A0A3}"/>
   </bookViews>
   <sheets>
     <sheet name="name" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Re 01" sheetId="3" r:id="rId3"/>
     <sheet name="Re 02" sheetId="4" r:id="rId4"/>
     <sheet name="Exe 16 - axb" sheetId="5" r:id="rId5"/>
+    <sheet name="Exe 17 - Find number" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="194">
   <si>
     <t>構成</t>
   </si>
@@ -623,12 +624,93 @@
       <t xml:space="preserve"> chuỗi text hay không. So sánh từ ngay vị trí bắt đầu</t>
     </r>
   </si>
+  <si>
+    <t>exe_17_find_number.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_17_find_number.py</t>
+  </si>
+  <si>
+    <t># Input     : Lấy các giá trị số trong một chuỗi và đưa vào 1 list</t>
+  </si>
+  <si>
+    <t># Output    : [1,2,10]</t>
+  </si>
+  <si>
+    <t># Ví dụ     : Exercises number 1, 12, 13, and 345 are important</t>
+  </si>
+  <si>
+    <t># Ví dụ     : [1, 12, 13, 345]</t>
+  </si>
+  <si>
+    <t>text    = "Exercises number 19, 12, 13, and 345 are important"</t>
+  </si>
+  <si>
+    <t>listResult = []</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    listResult.append(int(n.group()) )</t>
+  </si>
+  <si>
+    <t>print(listResult)</t>
+  </si>
+  <si>
+    <t>python3 exe_17_find_number.py</t>
+  </si>
+  <si>
+    <t>for n in re.finditer("[0-9]{1,}", text)::</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">span là chỉ số xuất hiện của của </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>123 abc xabc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">. Để lấy được giá trị </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">123 abc xabc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">thì mình cần dùng phương thức </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>group()</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -661,6 +743,11 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
@@ -1872,6 +1959,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>67733</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257210</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>33867</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5529D0B-DB5B-2A37-0C94-F9FEE7AA69DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="905932" y="21403733"/>
+          <a:ext cx="10137811" cy="982134"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4424,8 +4560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF812D9-6BE9-D24E-A2E0-24511D7FDF00}">
   <dimension ref="A3:O182"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="125" workbookViewId="0">
-      <selection activeCell="M98" sqref="M98"/>
+    <sheetView topLeftCell="C110" zoomScale="125" workbookViewId="0">
+      <selection activeCell="R136" sqref="R136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5767,6 +5903,12 @@
       <c r="B129" s="15"/>
       <c r="K129" s="16"/>
       <c r="L129" s="16"/>
+      <c r="M129" t="s">
+        <v>71</v>
+      </c>
+      <c r="N129" t="s">
+        <v>193</v>
+      </c>
       <c r="O129" s="16"/>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.2">
@@ -8134,8 +8276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DAD38-D54D-9F45-8003-4333ED54CE92}">
   <dimension ref="A3:M117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="191" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView zoomScale="191" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8706,7 +8848,7 @@
       <c r="A56" s="1"/>
       <c r="B56" s="5"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="26" t="s">
+      <c r="D56" t="s">
         <v>137</v>
       </c>
       <c r="E56" s="1"/>
@@ -8717,7 +8859,7 @@
       <c r="A57" s="1"/>
       <c r="B57" s="5"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="26" t="s">
+      <c r="D57" t="s">
         <v>144</v>
       </c>
       <c r="E57" s="1"/>
@@ -8728,7 +8870,7 @@
       <c r="A58" s="1"/>
       <c r="B58" s="5"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="26" t="s">
+      <c r="D58" t="s">
         <v>159</v>
       </c>
       <c r="E58" s="1"/>
@@ -9047,10 +9189,6 @@
       <c r="F88" s="13"/>
       <c r="G88" s="13"/>
       <c r="H88" s="14"/>
-      <c r="I88" s="27"/>
-      <c r="J88" s="27"/>
-      <c r="K88" s="27"/>
-      <c r="L88" s="27"/>
       <c r="M88" s="16"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
@@ -9058,16 +9196,7 @@
       <c r="B89" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
       <c r="H89" s="16"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-      <c r="K89" s="27"/>
-      <c r="L89" s="27"/>
       <c r="M89" s="16"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
@@ -9075,31 +9204,13 @@
       <c r="B90" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
-      <c r="E90" s="27"/>
-      <c r="F90" s="27"/>
-      <c r="G90" s="27"/>
       <c r="H90" s="16"/>
-      <c r="I90" s="27"/>
-      <c r="J90" s="27"/>
-      <c r="K90" s="27"/>
-      <c r="L90" s="27"/>
       <c r="M90" s="16"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="15"/>
       <c r="B91" s="15"/>
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="27"/>
       <c r="H91" s="16"/>
-      <c r="I91" s="27"/>
-      <c r="J91" s="27"/>
-      <c r="K91" s="27"/>
-      <c r="L91" s="27"/>
       <c r="M91" s="16"/>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
@@ -9107,16 +9218,7 @@
       <c r="B92" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="27"/>
       <c r="H92" s="16"/>
-      <c r="I92" s="27"/>
-      <c r="J92" s="27"/>
-      <c r="K92" s="27"/>
-      <c r="L92" s="27"/>
       <c r="M92" s="16"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
@@ -9124,16 +9226,7 @@
       <c r="B93" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
       <c r="H93" s="16"/>
-      <c r="I93" s="27"/>
-      <c r="J93" s="27"/>
-      <c r="K93" s="27"/>
-      <c r="L93" s="27"/>
       <c r="M93" s="16"/>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
@@ -9141,20 +9234,13 @@
       <c r="B94" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
-      <c r="F94" s="27"/>
-      <c r="G94" s="27"/>
       <c r="H94" s="16"/>
-      <c r="I94" s="27" t="s">
+      <c r="I94" t="s">
         <v>71</v>
       </c>
-      <c r="J94" s="27" t="s">
+      <c r="J94" t="s">
         <v>178</v>
       </c>
-      <c r="K94" s="27"/>
-      <c r="L94" s="27"/>
       <c r="M94" s="16"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
@@ -9162,16 +9248,7 @@
       <c r="B95" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="C95" s="27"/>
-      <c r="D95" s="27"/>
-      <c r="E95" s="27"/>
-      <c r="F95" s="27"/>
-      <c r="G95" s="27"/>
       <c r="H95" s="16"/>
-      <c r="I95" s="27"/>
-      <c r="J95" s="27"/>
-      <c r="K95" s="27"/>
-      <c r="L95" s="27"/>
       <c r="M95" s="16"/>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -9179,16 +9256,7 @@
       <c r="B96" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27"/>
-      <c r="F96" s="27"/>
-      <c r="G96" s="27"/>
       <c r="H96" s="16"/>
-      <c r="I96" s="27"/>
-      <c r="J96" s="27"/>
-      <c r="K96" s="27"/>
-      <c r="L96" s="27"/>
       <c r="M96" s="16"/>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
@@ -9196,16 +9264,7 @@
       <c r="B97" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
       <c r="H97" s="16"/>
-      <c r="I97" s="27"/>
-      <c r="J97" s="27"/>
-      <c r="K97" s="27"/>
-      <c r="L97" s="27"/>
       <c r="M97" s="16"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
@@ -9213,31 +9272,13 @@
       <c r="B98" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
       <c r="H98" s="16"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="27"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="27"/>
       <c r="M98" s="16"/>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="15"/>
       <c r="B99" s="15"/>
-      <c r="C99" s="27"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="27"/>
       <c r="H99" s="16"/>
-      <c r="I99" s="27"/>
-      <c r="J99" s="27"/>
-      <c r="K99" s="27"/>
-      <c r="L99" s="27"/>
       <c r="M99" s="16"/>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
@@ -9245,16 +9286,7 @@
       <c r="B100" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27"/>
-      <c r="F100" s="27"/>
-      <c r="G100" s="27"/>
       <c r="H100" s="16"/>
-      <c r="I100" s="27"/>
-      <c r="J100" s="27"/>
-      <c r="K100" s="27"/>
-      <c r="L100" s="27"/>
       <c r="M100" s="16"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
@@ -9262,16 +9294,7 @@
       <c r="B101" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="C101" s="27"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="27"/>
-      <c r="F101" s="27"/>
-      <c r="G101" s="27"/>
       <c r="H101" s="16"/>
-      <c r="I101" s="27"/>
-      <c r="J101" s="27"/>
-      <c r="K101" s="27"/>
-      <c r="L101" s="27"/>
       <c r="M101" s="16"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
@@ -9279,16 +9302,7 @@
       <c r="B102" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="C102" s="27"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="27"/>
       <c r="H102" s="16"/>
-      <c r="I102" s="27"/>
-      <c r="J102" s="27"/>
-      <c r="K102" s="27"/>
-      <c r="L102" s="27"/>
       <c r="M102" s="16"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -9296,16 +9310,7 @@
       <c r="B103" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="27"/>
-      <c r="G103" s="27"/>
       <c r="H103" s="16"/>
-      <c r="I103" s="27"/>
-      <c r="J103" s="27"/>
-      <c r="K103" s="27"/>
-      <c r="L103" s="27"/>
       <c r="M103" s="16"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -9313,16 +9318,7 @@
       <c r="B104" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C104" s="27"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27"/>
-      <c r="F104" s="27"/>
-      <c r="G104" s="27"/>
       <c r="H104" s="16"/>
-      <c r="I104" s="27"/>
-      <c r="J104" s="27"/>
-      <c r="K104" s="27"/>
-      <c r="L104" s="27"/>
       <c r="M104" s="16"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
@@ -9334,40 +9330,14 @@
       <c r="F105" s="18"/>
       <c r="G105" s="18"/>
       <c r="H105" s="19"/>
-      <c r="I105" s="27"/>
-      <c r="J105" s="27"/>
-      <c r="K105" s="27"/>
-      <c r="L105" s="27"/>
       <c r="M105" s="16"/>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="15"/>
-      <c r="B106" s="27"/>
-      <c r="C106" s="27"/>
-      <c r="D106" s="27"/>
-      <c r="E106" s="27"/>
-      <c r="F106" s="27"/>
-      <c r="G106" s="27"/>
-      <c r="H106" s="27"/>
-      <c r="I106" s="27"/>
-      <c r="J106" s="27"/>
-      <c r="K106" s="27"/>
-      <c r="L106" s="27"/>
       <c r="M106" s="16"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="15"/>
-      <c r="B107" s="27"/>
-      <c r="C107" s="27"/>
-      <c r="D107" s="27"/>
-      <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
-      <c r="G107" s="27"/>
-      <c r="H107" s="27"/>
-      <c r="I107" s="27"/>
-      <c r="J107" s="27"/>
-      <c r="K107" s="27"/>
-      <c r="L107" s="27"/>
       <c r="M107" s="16"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -9390,105 +9360,42 @@
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="15"/>
       <c r="B109" s="15"/>
-      <c r="C109" s="27"/>
-      <c r="D109" s="27"/>
-      <c r="E109" s="27"/>
-      <c r="F109" s="27"/>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
-      <c r="I109" s="27"/>
-      <c r="J109" s="27"/>
-      <c r="K109" s="27"/>
       <c r="L109" s="16"/>
       <c r="M109" s="16"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="15"/>
       <c r="B110" s="15"/>
-      <c r="C110" s="27"/>
-      <c r="D110" s="27"/>
-      <c r="E110" s="27"/>
-      <c r="F110" s="27"/>
-      <c r="G110" s="27"/>
-      <c r="H110" s="27"/>
-      <c r="I110" s="27"/>
-      <c r="J110" s="27"/>
-      <c r="K110" s="27"/>
       <c r="L110" s="16"/>
       <c r="M110" s="16"/>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="15"/>
       <c r="B111" s="15"/>
-      <c r="C111" s="27"/>
-      <c r="D111" s="27"/>
-      <c r="E111" s="27"/>
-      <c r="F111" s="27"/>
-      <c r="G111" s="27"/>
-      <c r="H111" s="27"/>
-      <c r="I111" s="27"/>
-      <c r="J111" s="27"/>
-      <c r="K111" s="27"/>
       <c r="L111" s="16"/>
       <c r="M111" s="16"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="15"/>
       <c r="B112" s="15"/>
-      <c r="C112" s="27"/>
-      <c r="D112" s="27"/>
-      <c r="E112" s="27"/>
-      <c r="F112" s="27"/>
-      <c r="G112" s="27"/>
-      <c r="H112" s="27"/>
-      <c r="I112" s="27"/>
-      <c r="J112" s="27"/>
-      <c r="K112" s="27"/>
       <c r="L112" s="16"/>
       <c r="M112" s="16"/>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" s="15"/>
       <c r="B113" s="15"/>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27"/>
-      <c r="E113" s="27"/>
-      <c r="F113" s="27"/>
-      <c r="G113" s="27"/>
-      <c r="H113" s="27"/>
-      <c r="I113" s="27"/>
-      <c r="J113" s="27"/>
-      <c r="K113" s="27"/>
       <c r="L113" s="16"/>
       <c r="M113" s="16"/>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="15"/>
       <c r="B114" s="15"/>
-      <c r="C114" s="27"/>
-      <c r="D114" s="27"/>
-      <c r="E114" s="27"/>
-      <c r="F114" s="27"/>
-      <c r="G114" s="27"/>
-      <c r="H114" s="27"/>
-      <c r="I114" s="27"/>
-      <c r="J114" s="27"/>
-      <c r="K114" s="27"/>
       <c r="L114" s="16"/>
       <c r="M114" s="16"/>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="15"/>
       <c r="B115" s="15"/>
-      <c r="C115" s="27"/>
-      <c r="D115" s="27"/>
-      <c r="E115" s="27"/>
-      <c r="F115" s="27"/>
-      <c r="G115" s="27"/>
-      <c r="H115" s="27"/>
-      <c r="I115" s="27"/>
-      <c r="J115" s="27"/>
-      <c r="K115" s="27"/>
       <c r="L115" s="16"/>
       <c r="M115" s="16"/>
     </row>
@@ -9526,4 +9433,1358 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F8EFF0-244C-3247-9FA3-E2853E03B0E8}">
+  <dimension ref="A3:O112"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="1"/>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="1"/>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="1"/>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="5"/>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="5"/>
+      <c r="D39" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="5"/>
+      <c r="D40" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="5"/>
+      <c r="D41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="1"/>
+      <c r="D43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="1"/>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="1"/>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="1"/>
+      <c r="D46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="1"/>
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="1"/>
+      <c r="D48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="1"/>
+      <c r="D49" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="1"/>
+      <c r="D50" t="s">
+        <v>47</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="1"/>
+      <c r="D52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="1"/>
+      <c r="D53" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="1"/>
+      <c r="D54" t="s">
+        <v>111</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="1"/>
+      <c r="D55" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="1"/>
+      <c r="D56" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="1"/>
+      <c r="D57" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="1"/>
+      <c r="D58" t="s">
+        <v>159</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="1"/>
+      <c r="D59" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="1"/>
+      <c r="D62" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="1"/>
+      <c r="D63" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="1"/>
+      <c r="D64" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="1"/>
+      <c r="D65" t="s">
+        <v>53</v>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="1"/>
+      <c r="D66" t="s">
+        <v>54</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="5"/>
+      <c r="C80" t="s">
+        <v>68</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="5"/>
+      <c r="C81" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="B82" s="5"/>
+      <c r="C82" t="s">
+        <v>70</v>
+      </c>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H84" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="1"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A88" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+      <c r="K88" s="13"/>
+      <c r="L88" s="13"/>
+      <c r="M88" s="13"/>
+      <c r="N88" s="13"/>
+      <c r="O88" s="14"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A89" s="15"/>
+      <c r="B89" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="27"/>
+      <c r="I89" s="27"/>
+      <c r="J89" s="27"/>
+      <c r="K89" s="27"/>
+      <c r="L89" s="27"/>
+      <c r="M89" s="27"/>
+      <c r="N89" s="27"/>
+      <c r="O89" s="16"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A90" s="15"/>
+      <c r="B90" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C90" s="27"/>
+      <c r="D90" s="27"/>
+      <c r="E90" s="27"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="27"/>
+      <c r="H90" s="27"/>
+      <c r="I90" s="27"/>
+      <c r="J90" s="27"/>
+      <c r="K90" s="27"/>
+      <c r="L90" s="27"/>
+      <c r="M90" s="27"/>
+      <c r="N90" s="27"/>
+      <c r="O90" s="16"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A91" s="15"/>
+      <c r="B91" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="27"/>
+      <c r="H91" s="27"/>
+      <c r="I91" s="27"/>
+      <c r="J91" s="27"/>
+      <c r="K91" s="27"/>
+      <c r="L91" s="27"/>
+      <c r="M91" s="27"/>
+      <c r="N91" s="27"/>
+      <c r="O91" s="16"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A92" s="15"/>
+      <c r="B92" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="27"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="27"/>
+      <c r="H92" s="27"/>
+      <c r="I92" s="27"/>
+      <c r="J92" s="27"/>
+      <c r="K92" s="27"/>
+      <c r="L92" s="27"/>
+      <c r="M92" s="27"/>
+      <c r="N92" s="27"/>
+      <c r="O92" s="16"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A93" s="15"/>
+      <c r="B93" s="15"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="27"/>
+      <c r="H93" s="27"/>
+      <c r="I93" s="27"/>
+      <c r="J93" s="27"/>
+      <c r="K93" s="27"/>
+      <c r="L93" s="27"/>
+      <c r="M93" s="27"/>
+      <c r="N93" s="27"/>
+      <c r="O93" s="16"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A94" s="15"/>
+      <c r="B94" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="27"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="27"/>
+      <c r="H94" s="27"/>
+      <c r="I94" s="27"/>
+      <c r="J94" s="27"/>
+      <c r="K94" s="27"/>
+      <c r="L94" s="27"/>
+      <c r="M94" s="27"/>
+      <c r="N94" s="27"/>
+      <c r="O94" s="16"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A95" s="15"/>
+      <c r="B95" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="27"/>
+      <c r="H95" s="27"/>
+      <c r="I95" s="27"/>
+      <c r="J95" s="27"/>
+      <c r="K95" s="27"/>
+      <c r="L95" s="27"/>
+      <c r="M95" s="27"/>
+      <c r="N95" s="27"/>
+      <c r="O95" s="16"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A96" s="15"/>
+      <c r="B96" s="15"/>
+      <c r="C96" s="27"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="27"/>
+      <c r="H96" s="27"/>
+      <c r="I96" s="27"/>
+      <c r="J96" s="27"/>
+      <c r="K96" s="27"/>
+      <c r="L96" s="27"/>
+      <c r="M96" s="27"/>
+      <c r="N96" s="27"/>
+      <c r="O96" s="16"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A97" s="15"/>
+      <c r="B97" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C97" s="27"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="27"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="27"/>
+      <c r="H97" s="27"/>
+      <c r="I97" s="27"/>
+      <c r="J97" s="27"/>
+      <c r="K97" s="27"/>
+      <c r="L97" s="27"/>
+      <c r="M97" s="27"/>
+      <c r="N97" s="27"/>
+      <c r="O97" s="16"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A98" s="15"/>
+      <c r="B98" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="27"/>
+      <c r="H98" s="27"/>
+      <c r="I98" s="27"/>
+      <c r="J98" s="27"/>
+      <c r="K98" s="27"/>
+      <c r="L98" s="27"/>
+      <c r="M98" s="27"/>
+      <c r="N98" s="27"/>
+      <c r="O98" s="16"/>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A99" s="15"/>
+      <c r="B99" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C99" s="27"/>
+      <c r="D99" s="27"/>
+      <c r="E99" s="27"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="27"/>
+      <c r="H99" s="27"/>
+      <c r="I99" s="27"/>
+      <c r="J99" s="27"/>
+      <c r="K99" s="27"/>
+      <c r="L99" s="27"/>
+      <c r="M99" s="27"/>
+      <c r="N99" s="27"/>
+      <c r="O99" s="16"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A100" s="15"/>
+      <c r="B100" s="15"/>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="16"/>
+      <c r="G100" s="27"/>
+      <c r="H100" s="27"/>
+      <c r="I100" s="27"/>
+      <c r="J100" s="27"/>
+      <c r="K100" s="27"/>
+      <c r="L100" s="27"/>
+      <c r="M100" s="27"/>
+      <c r="N100" s="27"/>
+      <c r="O100" s="16"/>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A101" s="15"/>
+      <c r="B101" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="27"/>
+      <c r="H101" s="27"/>
+      <c r="I101" s="27"/>
+      <c r="J101" s="27"/>
+      <c r="K101" s="27"/>
+      <c r="L101" s="27"/>
+      <c r="M101" s="27"/>
+      <c r="N101" s="27"/>
+      <c r="O101" s="16"/>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A102" s="15"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="19"/>
+      <c r="G102" s="27"/>
+      <c r="H102" s="27"/>
+      <c r="I102" s="27"/>
+      <c r="J102" s="27"/>
+      <c r="K102" s="27"/>
+      <c r="L102" s="27"/>
+      <c r="M102" s="27"/>
+      <c r="N102" s="27"/>
+      <c r="O102" s="16"/>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A103" s="15"/>
+      <c r="B103" s="27"/>
+      <c r="C103" s="27"/>
+      <c r="D103" s="27"/>
+      <c r="E103" s="27"/>
+      <c r="F103" s="27"/>
+      <c r="G103" s="27"/>
+      <c r="H103" s="27"/>
+      <c r="I103" s="27"/>
+      <c r="J103" s="27"/>
+      <c r="K103" s="27"/>
+      <c r="L103" s="27"/>
+      <c r="M103" s="27"/>
+      <c r="N103" s="27"/>
+      <c r="O103" s="16"/>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A104" s="15"/>
+      <c r="B104" s="27"/>
+      <c r="C104" s="27"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="27"/>
+      <c r="G104" s="27"/>
+      <c r="H104" s="27"/>
+      <c r="I104" s="27"/>
+      <c r="J104" s="27"/>
+      <c r="K104" s="27"/>
+      <c r="L104" s="27"/>
+      <c r="M104" s="27"/>
+      <c r="N104" s="27"/>
+      <c r="O104" s="16"/>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A105" s="15"/>
+      <c r="B105" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C105" s="13"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="13"/>
+      <c r="I105" s="13"/>
+      <c r="J105" s="13"/>
+      <c r="K105" s="13"/>
+      <c r="L105" s="13"/>
+      <c r="M105" s="13"/>
+      <c r="N105" s="14"/>
+      <c r="O105" s="16"/>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A106" s="15"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="27"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="27"/>
+      <c r="H106" s="27"/>
+      <c r="I106" s="27"/>
+      <c r="J106" s="27"/>
+      <c r="K106" s="27"/>
+      <c r="L106" s="27"/>
+      <c r="M106" s="27"/>
+      <c r="N106" s="16"/>
+      <c r="O106" s="16"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A107" s="15"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="27"/>
+      <c r="G107" s="27"/>
+      <c r="H107" s="27"/>
+      <c r="I107" s="27"/>
+      <c r="J107" s="27"/>
+      <c r="K107" s="27"/>
+      <c r="L107" s="27"/>
+      <c r="M107" s="27"/>
+      <c r="N107" s="16"/>
+      <c r="O107" s="16"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A108" s="15"/>
+      <c r="B108" s="15"/>
+      <c r="C108" s="27"/>
+      <c r="D108" s="27"/>
+      <c r="E108" s="27"/>
+      <c r="F108" s="27"/>
+      <c r="G108" s="27"/>
+      <c r="H108" s="27"/>
+      <c r="I108" s="27"/>
+      <c r="J108" s="27"/>
+      <c r="K108" s="27"/>
+      <c r="L108" s="27"/>
+      <c r="M108" s="27"/>
+      <c r="N108" s="16"/>
+      <c r="O108" s="16"/>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A109" s="15"/>
+      <c r="B109" s="15"/>
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="27"/>
+      <c r="I109" s="27"/>
+      <c r="J109" s="27"/>
+      <c r="K109" s="27"/>
+      <c r="L109" s="27"/>
+      <c r="M109" s="27"/>
+      <c r="N109" s="16"/>
+      <c r="O109" s="16"/>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A110" s="15"/>
+      <c r="B110" s="15"/>
+      <c r="C110" s="27"/>
+      <c r="D110" s="27"/>
+      <c r="E110" s="27"/>
+      <c r="F110" s="27"/>
+      <c r="G110" s="27"/>
+      <c r="H110" s="27"/>
+      <c r="I110" s="27"/>
+      <c r="J110" s="27"/>
+      <c r="K110" s="27"/>
+      <c r="L110" s="27"/>
+      <c r="M110" s="27"/>
+      <c r="N110" s="16"/>
+      <c r="O110" s="16"/>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A111" s="15"/>
+      <c r="B111" s="17"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="18"/>
+      <c r="F111" s="18"/>
+      <c r="G111" s="18"/>
+      <c r="H111" s="18"/>
+      <c r="I111" s="18"/>
+      <c r="J111" s="18"/>
+      <c r="K111" s="18"/>
+      <c r="L111" s="18"/>
+      <c r="M111" s="18"/>
+      <c r="N111" s="19"/>
+      <c r="O111" s="16"/>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A112" s="17"/>
+      <c r="B112" s="18"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+      <c r="H112" s="18"/>
+      <c r="I112" s="18"/>
+      <c r="J112" s="18"/>
+      <c r="K112" s="18"/>
+      <c r="L112" s="18"/>
+      <c r="M112" s="18"/>
+      <c r="N112" s="18"/>
+      <c r="O112" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exe 18 - street
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/9.Cac-van-de-mo-rong.xlsx
+++ b/me/1.Lap-trinh-python/9.Cac-van-de-mo-rong.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFA057D-FD60-6649-8DCD-962AD7254D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E4CAF1-F33D-4D46-9B6C-A7422F5187C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="820" windowWidth="33800" windowHeight="18400" activeTab="5" xr2:uid="{472041F3-94B6-BA44-8755-3BBFF041A0A3}"/>
+    <workbookView xWindow="1120" yWindow="1400" windowWidth="33800" windowHeight="18000" activeTab="6" xr2:uid="{472041F3-94B6-BA44-8755-3BBFF041A0A3}"/>
   </bookViews>
   <sheets>
     <sheet name="name" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Re 02" sheetId="4" r:id="rId4"/>
     <sheet name="Exe 16 - axb" sheetId="5" r:id="rId5"/>
     <sheet name="Exe 17 - Find number" sheetId="6" r:id="rId6"/>
+    <sheet name="Exe 18 - street" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="210">
   <si>
     <t>構成</t>
   </si>
@@ -704,6 +705,104 @@
       </rPr>
       <t>group()</t>
     </r>
+  </si>
+  <si>
+    <t>exe_18_street.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_18_street.py</t>
+  </si>
+  <si>
+    <t># Input     : Chuỗi địa chỉ kết thúc với từ street</t>
+  </si>
+  <si>
+    <t># Output    : thay từ street thành st.</t>
+  </si>
+  <si>
+    <t># Ví dụ     : 21 To Hien Thanh street</t>
+  </si>
+  <si>
+    <t># Ví dụ     : 21 To Hien Thanh sTREet</t>
+  </si>
+  <si>
+    <t># Ví dụ     : 21 To Hien Thanh st.</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>python3 exe_18_street.py</t>
+  </si>
+  <si>
+    <t>Trường hợp có chữ in hoa thì vẫn tự động thay thế được</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inputText = '21 To Hien Thanh </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>street</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inputText = '21 To Hien Thanh </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>strEet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">21 To Hien Thanh </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>st.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">flags= re.I </t>
+  </si>
+  <si>
+    <t>Không phân biệt hoa và thường</t>
+  </si>
+  <si>
+    <t>result  = re.sub('street$', 'st.', inputText, flags= re.I) # flags=re.I</t>
   </si>
 </sst>
 </file>
@@ -2008,6 +2107,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>92235</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>78044</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>149207</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>35475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C22F5841-164A-8A7B-046D-61FE699A4887}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="915252" y="22299497"/>
+          <a:ext cx="9110156" cy="986201"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9439,8 +9587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F8EFF0-244C-3247-9FA3-E2853E03B0E8}">
   <dimension ref="A3:O112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H92" sqref="H92"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10302,7 +10450,7 @@
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="5"/>
-      <c r="C83" s="26" t="s">
+      <c r="C83" t="s">
         <v>161</v>
       </c>
       <c r="D83" s="1"/>
@@ -10362,14 +10510,6 @@
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
       <c r="F89" s="14"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-      <c r="K89" s="27"/>
-      <c r="L89" s="27"/>
-      <c r="M89" s="27"/>
-      <c r="N89" s="27"/>
       <c r="O89" s="16"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
@@ -10377,18 +10517,7 @@
       <c r="B90" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
-      <c r="E90" s="27"/>
       <c r="F90" s="16"/>
-      <c r="G90" s="27"/>
-      <c r="H90" s="27"/>
-      <c r="I90" s="27"/>
-      <c r="J90" s="27"/>
-      <c r="K90" s="27"/>
-      <c r="L90" s="27"/>
-      <c r="M90" s="27"/>
-      <c r="N90" s="27"/>
       <c r="O90" s="16"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
@@ -10396,18 +10525,7 @@
       <c r="B91" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27"/>
       <c r="F91" s="16"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="27"/>
-      <c r="I91" s="27"/>
-      <c r="J91" s="27"/>
-      <c r="K91" s="27"/>
-      <c r="L91" s="27"/>
-      <c r="M91" s="27"/>
-      <c r="N91" s="27"/>
       <c r="O91" s="16"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
@@ -10415,35 +10533,13 @@
       <c r="B92" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
       <c r="F92" s="16"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="27"/>
-      <c r="I92" s="27"/>
-      <c r="J92" s="27"/>
-      <c r="K92" s="27"/>
-      <c r="L92" s="27"/>
-      <c r="M92" s="27"/>
-      <c r="N92" s="27"/>
       <c r="O92" s="16"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="15"/>
       <c r="B93" s="15"/>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
       <c r="F93" s="16"/>
-      <c r="G93" s="27"/>
-      <c r="H93" s="27"/>
-      <c r="I93" s="27"/>
-      <c r="J93" s="27"/>
-      <c r="K93" s="27"/>
-      <c r="L93" s="27"/>
-      <c r="M93" s="27"/>
-      <c r="N93" s="27"/>
       <c r="O93" s="16"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
@@ -10451,18 +10547,7 @@
       <c r="B94" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
       <c r="F94" s="16"/>
-      <c r="G94" s="27"/>
-      <c r="H94" s="27"/>
-      <c r="I94" s="27"/>
-      <c r="J94" s="27"/>
-      <c r="K94" s="27"/>
-      <c r="L94" s="27"/>
-      <c r="M94" s="27"/>
-      <c r="N94" s="27"/>
       <c r="O94" s="16"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
@@ -10470,35 +10555,13 @@
       <c r="B95" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="C95" s="27"/>
-      <c r="D95" s="27"/>
-      <c r="E95" s="27"/>
       <c r="F95" s="16"/>
-      <c r="G95" s="27"/>
-      <c r="H95" s="27"/>
-      <c r="I95" s="27"/>
-      <c r="J95" s="27"/>
-      <c r="K95" s="27"/>
-      <c r="L95" s="27"/>
-      <c r="M95" s="27"/>
-      <c r="N95" s="27"/>
       <c r="O95" s="16"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="15"/>
       <c r="B96" s="15"/>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27"/>
       <c r="F96" s="16"/>
-      <c r="G96" s="27"/>
-      <c r="H96" s="27"/>
-      <c r="I96" s="27"/>
-      <c r="J96" s="27"/>
-      <c r="K96" s="27"/>
-      <c r="L96" s="27"/>
-      <c r="M96" s="27"/>
-      <c r="N96" s="27"/>
       <c r="O96" s="16"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
@@ -10506,18 +10569,7 @@
       <c r="B97" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
       <c r="F97" s="16"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="27"/>
-      <c r="I97" s="27"/>
-      <c r="J97" s="27"/>
-      <c r="K97" s="27"/>
-      <c r="L97" s="27"/>
-      <c r="M97" s="27"/>
-      <c r="N97" s="27"/>
       <c r="O97" s="16"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
@@ -10525,18 +10577,7 @@
       <c r="B98" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
       <c r="F98" s="16"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="27"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="27"/>
-      <c r="M98" s="27"/>
-      <c r="N98" s="27"/>
       <c r="O98" s="16"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
@@ -10544,35 +10585,13 @@
       <c r="B99" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="C99" s="27"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
       <c r="F99" s="16"/>
-      <c r="G99" s="27"/>
-      <c r="H99" s="27"/>
-      <c r="I99" s="27"/>
-      <c r="J99" s="27"/>
-      <c r="K99" s="27"/>
-      <c r="L99" s="27"/>
-      <c r="M99" s="27"/>
-      <c r="N99" s="27"/>
       <c r="O99" s="16"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" s="15"/>
       <c r="B100" s="15"/>
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27"/>
       <c r="F100" s="16"/>
-      <c r="G100" s="27"/>
-      <c r="H100" s="27"/>
-      <c r="I100" s="27"/>
-      <c r="J100" s="27"/>
-      <c r="K100" s="27"/>
-      <c r="L100" s="27"/>
-      <c r="M100" s="27"/>
-      <c r="N100" s="27"/>
       <c r="O100" s="16"/>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.2">
@@ -10580,18 +10599,7 @@
       <c r="B101" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="C101" s="27"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="27"/>
       <c r="F101" s="16"/>
-      <c r="G101" s="27"/>
-      <c r="H101" s="27"/>
-      <c r="I101" s="27"/>
-      <c r="J101" s="27"/>
-      <c r="K101" s="27"/>
-      <c r="L101" s="27"/>
-      <c r="M101" s="27"/>
-      <c r="N101" s="27"/>
       <c r="O101" s="16"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
@@ -10601,48 +10609,14 @@
       <c r="D102" s="18"/>
       <c r="E102" s="18"/>
       <c r="F102" s="19"/>
-      <c r="G102" s="27"/>
-      <c r="H102" s="27"/>
-      <c r="I102" s="27"/>
-      <c r="J102" s="27"/>
-      <c r="K102" s="27"/>
-      <c r="L102" s="27"/>
-      <c r="M102" s="27"/>
-      <c r="N102" s="27"/>
       <c r="O102" s="16"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="15"/>
-      <c r="B103" s="27"/>
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="27"/>
-      <c r="G103" s="27"/>
-      <c r="H103" s="27"/>
-      <c r="I103" s="27"/>
-      <c r="J103" s="27"/>
-      <c r="K103" s="27"/>
-      <c r="L103" s="27"/>
-      <c r="M103" s="27"/>
-      <c r="N103" s="27"/>
       <c r="O103" s="16"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="15"/>
-      <c r="B104" s="27"/>
-      <c r="C104" s="27"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27"/>
-      <c r="F104" s="27"/>
-      <c r="G104" s="27"/>
-      <c r="H104" s="27"/>
-      <c r="I104" s="27"/>
-      <c r="J104" s="27"/>
-      <c r="K104" s="27"/>
-      <c r="L104" s="27"/>
-      <c r="M104" s="27"/>
-      <c r="N104" s="27"/>
       <c r="O104" s="16"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
@@ -10667,85 +10641,30 @@
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="15"/>
       <c r="B106" s="15"/>
-      <c r="C106" s="27"/>
-      <c r="D106" s="27"/>
-      <c r="E106" s="27"/>
-      <c r="F106" s="27"/>
-      <c r="G106" s="27"/>
-      <c r="H106" s="27"/>
-      <c r="I106" s="27"/>
-      <c r="J106" s="27"/>
-      <c r="K106" s="27"/>
-      <c r="L106" s="27"/>
-      <c r="M106" s="27"/>
       <c r="N106" s="16"/>
       <c r="O106" s="16"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" s="15"/>
       <c r="B107" s="15"/>
-      <c r="C107" s="27"/>
-      <c r="D107" s="27"/>
-      <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
-      <c r="G107" s="27"/>
-      <c r="H107" s="27"/>
-      <c r="I107" s="27"/>
-      <c r="J107" s="27"/>
-      <c r="K107" s="27"/>
-      <c r="L107" s="27"/>
-      <c r="M107" s="27"/>
       <c r="N107" s="16"/>
       <c r="O107" s="16"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="15"/>
       <c r="B108" s="15"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="27"/>
-      <c r="I108" s="27"/>
-      <c r="J108" s="27"/>
-      <c r="K108" s="27"/>
-      <c r="L108" s="27"/>
-      <c r="M108" s="27"/>
       <c r="N108" s="16"/>
       <c r="O108" s="16"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="15"/>
       <c r="B109" s="15"/>
-      <c r="C109" s="27"/>
-      <c r="D109" s="27"/>
-      <c r="E109" s="27"/>
-      <c r="F109" s="27"/>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
-      <c r="I109" s="27"/>
-      <c r="J109" s="27"/>
-      <c r="K109" s="27"/>
-      <c r="L109" s="27"/>
-      <c r="M109" s="27"/>
       <c r="N109" s="16"/>
       <c r="O109" s="16"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="15"/>
       <c r="B110" s="15"/>
-      <c r="C110" s="27"/>
-      <c r="D110" s="27"/>
-      <c r="E110" s="27"/>
-      <c r="F110" s="27"/>
-      <c r="G110" s="27"/>
-      <c r="H110" s="27"/>
-      <c r="I110" s="27"/>
-      <c r="J110" s="27"/>
-      <c r="K110" s="27"/>
-      <c r="L110" s="27"/>
-      <c r="M110" s="27"/>
       <c r="N110" s="16"/>
       <c r="O110" s="16"/>
     </row>
@@ -10787,4 +10706,1214 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD6E85A-E224-734D-B6F6-CCF22A1D3A86}">
+  <dimension ref="A3:M114"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="179" workbookViewId="0">
+      <selection activeCell="H104" sqref="H104"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="1"/>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="1"/>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="1"/>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="5"/>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="5"/>
+      <c r="D39" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="5"/>
+      <c r="D40" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="5"/>
+      <c r="D41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="1"/>
+      <c r="D43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="1"/>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="1"/>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="1"/>
+      <c r="D46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="1"/>
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="1"/>
+      <c r="D48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="1"/>
+      <c r="D49" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="1"/>
+      <c r="D50" t="s">
+        <v>47</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="1"/>
+      <c r="D52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="1"/>
+      <c r="D53" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="1"/>
+      <c r="D54" t="s">
+        <v>111</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="1"/>
+      <c r="D55" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="1"/>
+      <c r="D56" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="1"/>
+      <c r="D57" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="1"/>
+      <c r="D58" t="s">
+        <v>159</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="1"/>
+      <c r="D59" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="1"/>
+      <c r="D62" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="1"/>
+      <c r="D63" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="1"/>
+      <c r="D64" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="1"/>
+      <c r="D65" t="s">
+        <v>53</v>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="1"/>
+      <c r="D66" t="s">
+        <v>54</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="5"/>
+      <c r="C80" t="s">
+        <v>68</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="5"/>
+      <c r="C81" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="B82" s="5"/>
+      <c r="C82" t="s">
+        <v>70</v>
+      </c>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="B83" s="5"/>
+      <c r="C83" t="s">
+        <v>161</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="6"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H85" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="1"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B90" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="14"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B91" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="16"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B92" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="27"/>
+      <c r="F92" s="27"/>
+      <c r="G92" s="16"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B93" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="27"/>
+      <c r="G93" s="16"/>
+      <c r="H93" t="s">
+        <v>71</v>
+      </c>
+      <c r="I93" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B94" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="27"/>
+      <c r="F94" s="27"/>
+      <c r="G94" s="16"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B95" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="27"/>
+      <c r="G95" s="16"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B96" s="15"/>
+      <c r="C96" s="27"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="27"/>
+      <c r="G96" s="16"/>
+    </row>
+    <row r="97" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B97" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C97" s="27"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="27"/>
+      <c r="F97" s="27"/>
+      <c r="G97" s="16"/>
+    </row>
+    <row r="98" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B98" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="16"/>
+    </row>
+    <row r="99" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B99" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C99" s="27"/>
+      <c r="D99" s="27"/>
+      <c r="E99" s="27"/>
+      <c r="F99" s="27"/>
+      <c r="G99" s="16"/>
+      <c r="H99" t="s">
+        <v>71</v>
+      </c>
+      <c r="I99" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="100" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B100" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="16"/>
+      <c r="I100" t="s">
+        <v>207</v>
+      </c>
+      <c r="J100" t="s">
+        <v>71</v>
+      </c>
+      <c r="K100" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="101" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B101" s="15"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="27"/>
+      <c r="G101" s="16"/>
+    </row>
+    <row r="102" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B102" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C102" s="27"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27"/>
+      <c r="G102" s="16"/>
+    </row>
+    <row r="103" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B103" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C103" s="27"/>
+      <c r="D103" s="27"/>
+      <c r="E103" s="27"/>
+      <c r="F103" s="27"/>
+      <c r="G103" s="16"/>
+      <c r="H103" t="s">
+        <v>71</v>
+      </c>
+      <c r="I103" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="104" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B104" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C104" s="27"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="27"/>
+      <c r="G104" s="16"/>
+      <c r="I104" t="s">
+        <v>207</v>
+      </c>
+      <c r="J104" t="s">
+        <v>71</v>
+      </c>
+      <c r="K104" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="105" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B105" s="17"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="19"/>
+    </row>
+    <row r="108" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B108" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="13"/>
+      <c r="K108" s="13"/>
+      <c r="L108" s="13"/>
+      <c r="M108" s="14"/>
+    </row>
+    <row r="109" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B109" s="15"/>
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="27"/>
+      <c r="I109" s="27"/>
+      <c r="J109" s="27"/>
+      <c r="K109" s="27"/>
+      <c r="L109" s="27"/>
+      <c r="M109" s="16"/>
+    </row>
+    <row r="110" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B110" s="15"/>
+      <c r="C110" s="27"/>
+      <c r="D110" s="27"/>
+      <c r="E110" s="27"/>
+      <c r="F110" s="27"/>
+      <c r="G110" s="27"/>
+      <c r="H110" s="27"/>
+      <c r="I110" s="27"/>
+      <c r="J110" s="27"/>
+      <c r="K110" s="27"/>
+      <c r="L110" s="27"/>
+      <c r="M110" s="16"/>
+    </row>
+    <row r="111" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B111" s="15"/>
+      <c r="C111" s="27"/>
+      <c r="D111" s="27"/>
+      <c r="E111" s="27"/>
+      <c r="F111" s="27"/>
+      <c r="G111" s="27"/>
+      <c r="H111" s="27"/>
+      <c r="I111" s="27"/>
+      <c r="J111" s="27"/>
+      <c r="K111" s="27"/>
+      <c r="L111" s="27"/>
+      <c r="M111" s="16"/>
+    </row>
+    <row r="112" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B112" s="15"/>
+      <c r="C112" s="27"/>
+      <c r="D112" s="27"/>
+      <c r="E112" s="27"/>
+      <c r="F112" s="27"/>
+      <c r="G112" s="27"/>
+      <c r="H112" s="27"/>
+      <c r="I112" s="27"/>
+      <c r="J112" s="27"/>
+      <c r="K112" s="27"/>
+      <c r="L112" s="27"/>
+      <c r="M112" s="16"/>
+    </row>
+    <row r="113" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B113" s="15"/>
+      <c r="C113" s="27"/>
+      <c r="D113" s="27"/>
+      <c r="E113" s="27"/>
+      <c r="F113" s="27"/>
+      <c r="G113" s="27"/>
+      <c r="H113" s="27"/>
+      <c r="I113" s="27"/>
+      <c r="J113" s="27"/>
+      <c r="K113" s="27"/>
+      <c r="L113" s="27"/>
+      <c r="M113" s="16"/>
+    </row>
+    <row r="114" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B114" s="17"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="18"/>
+      <c r="H114" s="18"/>
+      <c r="I114" s="18"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="18"/>
+      <c r="L114" s="18"/>
+      <c r="M114" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>